<commit_message>
Revert "Merge branch 'main' into MinsuDelveop"
This reverts commit 2d14dea693f53844283cdd645b13817550dbd855.
</commit_message>
<xml_diff>
--- a/Assets/Resources/GuideResources/GuideDB_day3.xlsx
+++ b/Assets/Resources/GuideResources/GuideDB_day3.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\행잉\Hanging\Assets\Resources\GuideResources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\행잉\Data\가이드창\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -150,6 +150,18 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>&lt;최상급 시민&gt;
+마르티네즈, 헤르난데즈, 로페즈, 산체스, 리베라, 러셀, 리처즈, 멘데즈, 헤일
+&lt;상급 시민&gt;
+가르시아, 루이스, 넬슨, 에드워즈, 필립스, 반즈, 제이콥스, 크로스, 프로이드
+&lt;중급 시민&gt;테일러, 화이트, 잭슨, 앤더슨, 로드리게즈, 알렌, 콜린스, 로저스, 레이놀즈, 보이드, 해리슨, 라모스, 가렛, 메디나, 다니엘, 델가도, 오르테가, 무디
+&lt;하급 시민&gt;
+스미스, 데이비스, 마틴, 그린, 페레즈, 하워드, 알렉산더, 마이어스, 디아즈, 스티븐스, 라일리, 루이즈, 라이언, 메이어, 산티아, 슈나이더, 모란, 하몬
+&lt;최하급 시민&gt;
+브라운, 그레이, 젠킨스, 왓슨, 오티즈, 로즈, 페르난데즈, 오브라이언, 프랜시스</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>1급: 살인 / 2급: 상해, 폭행, 강도 / 3급: 강간, 강제 추행 / 4급: 협박, 공갈, 사기 / 5급: 모욕</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -220,19 +232,6 @@
 최상급: 없음
 상급: 2급까지 사면 가능
 그 외: 3급까지 사면 가능</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;최상급 시민&gt;
-마르티네즈, 헤르난데즈, 로페즈, 산체스, 리베라, 러셀, 리처즈, 멘데즈, 헤일
-&lt;상급 시민&gt;
-가르시아, 루이스, 넬슨, 에드워즈, 필립스, 반즈, 제이콥스, 크로스, 프로이드
-&lt;중급 시민&gt;
-테일러, 화이트, 잭슨, 앤더슨, 로드리게즈, 알렌, 콜린스, 로저스, 레이놀즈, 보이드, 해리슨, 라모스, 가렛, 메디나, 다니엘, 델가도, 오르테가, 무디
-&lt;하급 시민&gt;
-스미스, 데이비스, 마틴, 그린, 페레즈, 하워드, 알렉산더, 마이어스, 디아즈, 스티븐스, 라일리, 루이즈, 라이언, 메이어, 산티아, 슈나이더, 모란, 하몬
-&lt;최하급 시민&gt;
-브라운, 그레이, 젠킨스, 왓슨, 오티즈, 로즈, 페르난데즈, 오브라이언, 프랜시스</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -568,8 +567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -801,7 +800,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="346.5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>3</v>
       </c>
@@ -809,7 +808,7 @@
         <v>28</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -834,7 +833,7 @@
         <v>28</v>
       </c>
       <c r="C19" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -859,7 +858,7 @@
         <v>28</v>
       </c>
       <c r="C21" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -870,13 +869,13 @@
         <v>27</v>
       </c>
       <c r="C22" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D22" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="66" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="148.5" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>3</v>
       </c>
@@ -884,7 +883,7 @@
         <v>28</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -901,7 +900,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="82.5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="165" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>3</v>
       </c>
@@ -909,7 +908,7 @@
         <v>28</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -920,13 +919,13 @@
         <v>27</v>
       </c>
       <c r="C26" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D26" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="99" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>3</v>
       </c>
@@ -934,7 +933,7 @@
         <v>28</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -951,7 +950,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="33" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>3</v>
       </c>
@@ -959,13 +958,13 @@
         <v>27</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D29" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="66" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="247.5" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>3</v>
       </c>
@@ -973,10 +972,10 @@
         <v>28</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>3</v>
       </c>
@@ -984,13 +983,13 @@
         <v>27</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D31" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" ht="33" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>3</v>
       </c>
@@ -998,13 +997,13 @@
         <v>27</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D32" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="181.5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" ht="409.5" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>3</v>
       </c>
@@ -1012,10 +1011,10 @@
         <v>28</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="33" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>3</v>
       </c>
@@ -1023,13 +1022,13 @@
         <v>27</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D34" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="115.5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" ht="363" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>3</v>
       </c>
@@ -1037,7 +1036,7 @@
         <v>28</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Auto stash before rebase of "main"
</commit_message>
<xml_diff>
--- a/Assets/Resources/GuideResources/GuideDB_day3.xlsx
+++ b/Assets/Resources/GuideResources/GuideDB_day3.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\행잉\Data\가이드창\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\행잉\Hanging\Assets\Resources\GuideResources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -150,18 +150,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>&lt;최상급 시민&gt;
-마르티네즈, 헤르난데즈, 로페즈, 산체스, 리베라, 러셀, 리처즈, 멘데즈, 헤일
-&lt;상급 시민&gt;
-가르시아, 루이스, 넬슨, 에드워즈, 필립스, 반즈, 제이콥스, 크로스, 프로이드
-&lt;중급 시민&gt;테일러, 화이트, 잭슨, 앤더슨, 로드리게즈, 알렌, 콜린스, 로저스, 레이놀즈, 보이드, 해리슨, 라모스, 가렛, 메디나, 다니엘, 델가도, 오르테가, 무디
-&lt;하급 시민&gt;
-스미스, 데이비스, 마틴, 그린, 페레즈, 하워드, 알렉산더, 마이어스, 디아즈, 스티븐스, 라일리, 루이즈, 라이언, 메이어, 산티아, 슈나이더, 모란, 하몬
-&lt;최하급 시민&gt;
-브라운, 그레이, 젠킨스, 왓슨, 오티즈, 로즈, 페르난데즈, 오브라이언, 프랜시스</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1급: 살인 / 2급: 상해, 폭행, 강도 / 3급: 강간, 강제 추행 / 4급: 협박, 공갈, 사기 / 5급: 모욕</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -232,6 +220,19 @@
 최상급: 없음
 상급: 2급까지 사면 가능
 그 외: 3급까지 사면 가능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;최상급 시민&gt;
+마르티네즈, 헤르난데즈, 로페즈, 산체스, 리베라, 러셀, 리처즈, 멘데즈, 헤일
+&lt;상급 시민&gt;
+가르시아, 루이스, 넬슨, 에드워즈, 필립스, 반즈, 제이콥스, 크로스, 프로이드
+&lt;중급 시민&gt;
+테일러, 화이트, 잭슨, 앤더슨, 로드리게즈, 알렌, 콜린스, 로저스, 레이놀즈, 보이드, 해리슨, 라모스, 가렛, 메디나, 다니엘, 델가도, 오르테가, 무디
+&lt;하급 시민&gt;
+스미스, 데이비스, 마틴, 그린, 페레즈, 하워드, 알렉산더, 마이어스, 디아즈, 스티븐스, 라일리, 루이즈, 라이언, 메이어, 산티아, 슈나이더, 모란, 하몬
+&lt;최하급 시민&gt;
+브라운, 그레이, 젠킨스, 왓슨, 오티즈, 로즈, 페르난데즈, 오브라이언, 프랜시스</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -567,8 +568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E36"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -800,7 +801,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="409.5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="346.5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>3</v>
       </c>
@@ -808,7 +809,7 @@
         <v>28</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -833,7 +834,7 @@
         <v>28</v>
       </c>
       <c r="C19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -858,7 +859,7 @@
         <v>28</v>
       </c>
       <c r="C21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -869,13 +870,13 @@
         <v>27</v>
       </c>
       <c r="C22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D22" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="148.5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="66" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>3</v>
       </c>
@@ -883,7 +884,7 @@
         <v>28</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
@@ -900,7 +901,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="165" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>3</v>
       </c>
@@ -908,7 +909,7 @@
         <v>28</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -919,13 +920,13 @@
         <v>27</v>
       </c>
       <c r="C26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D26" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="99" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>3</v>
       </c>
@@ -933,7 +934,7 @@
         <v>28</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -950,7 +951,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="33" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>3</v>
       </c>
@@ -958,13 +959,13 @@
         <v>27</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D29" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="247.5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="66" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>3</v>
       </c>
@@ -972,24 +973,24 @@
         <v>28</v>
       </c>
       <c r="C30" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>3</v>
+      </c>
+      <c r="B31" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A31">
-        <v>3</v>
-      </c>
-      <c r="B31" t="s">
-        <v>27</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="D31" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="33" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>3</v>
       </c>
@@ -997,13 +998,13 @@
         <v>27</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D32" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="409.5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" ht="181.5" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>3</v>
       </c>
@@ -1011,24 +1012,24 @@
         <v>28</v>
       </c>
       <c r="C33" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>3</v>
+      </c>
+      <c r="B34" t="s">
+        <v>27</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="33" x14ac:dyDescent="0.3">
-      <c r="A34">
-        <v>3</v>
-      </c>
-      <c r="B34" t="s">
-        <v>27</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>44</v>
       </c>
       <c r="D34" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="363" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" ht="115.5" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>3</v>
       </c>
@@ -1036,7 +1037,7 @@
         <v>28</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>